<commit_message>
Adaugat notebook aco. Link raport in readme. Rezultate aco optimizate in excell.
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iustin.petrisor\Documents\master\An2\aea_tsp_with_drone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azza/Workspace/FAC/SEM 3/AEA/aea_tsp_with_drone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54448F5-2A7D-4CEF-9BC7-1E3C06A17763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E99D89-6424-7043-A100-79B4F71C2639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>AG</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>ACO</t>
+  </si>
+  <si>
+    <t>ACO OPTIMIZAT</t>
   </si>
 </sst>
 </file>
@@ -133,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -145,7 +151,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -158,21 +166,30 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -182,9 +199,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -196,32 +240,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -504,326 +535,1189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.5" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" customWidth="1"/>
+    <col min="12" max="12" width="4" customWidth="1"/>
+    <col min="15" max="15" width="4.1640625" customWidth="1"/>
+    <col min="18" max="18" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
         <v>112.298255214972</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9">
         <v>336.36589344233101</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9">
         <v>651.31643783594097</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="L3" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="M3" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="N3" s="12">
+        <v>249.07310752944301</v>
+      </c>
+      <c r="O3" s="12">
+        <v>249.07310752944301</v>
+      </c>
+      <c r="P3" s="12">
+        <v>249.07310752944301</v>
+      </c>
+      <c r="Q3" s="17">
+        <v>390.66091126679902</v>
+      </c>
+      <c r="R3" s="17">
+        <v>390.66091126679902</v>
+      </c>
+      <c r="S3" s="17">
+        <v>390.66091126679902</v>
+      </c>
+      <c r="T3" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="U3" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="V3" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="W3" s="12">
+        <v>177.97248805664199</v>
+      </c>
+      <c r="X3" s="12">
+        <v>177.97248805664199</v>
+      </c>
+      <c r="Y3" s="12">
+        <v>177.97248805664199</v>
+      </c>
+      <c r="Z3" s="12">
+        <v>299.88151301964501</v>
+      </c>
+      <c r="AA3" s="12">
+        <v>299.88151301964501</v>
+      </c>
+      <c r="AB3" s="12">
+        <v>299.88151301964501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>101.086110834465</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9">
         <v>346.24902424644199</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9">
         <v>661.83348648440199</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="L4" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="M4" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="N4" s="12">
+        <v>243.80745679595199</v>
+      </c>
+      <c r="O4" s="12">
+        <v>243.80745679595199</v>
+      </c>
+      <c r="P4" s="12">
+        <v>243.80745679595199</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>367.478757214437</v>
+      </c>
+      <c r="R4" s="17">
+        <v>367.478757214437</v>
+      </c>
+      <c r="S4" s="17">
+        <v>367.478757214437</v>
+      </c>
+      <c r="T4" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U4" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V4" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W4" s="12">
+        <v>184.19972188770399</v>
+      </c>
+      <c r="X4" s="12">
+        <v>184.19972188770399</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>184.19972188770399</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>291.22588160904797</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>291.22588160904797</v>
+      </c>
+      <c r="AB4" s="12">
+        <v>291.22588160904797</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="9">
         <v>108.30858975574201</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
         <v>345.24137954752302</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
         <v>677.34645258795103</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="12">
+        <v>104.502647181491</v>
+      </c>
+      <c r="L5" s="12">
+        <v>104.502647181491</v>
+      </c>
+      <c r="M5" s="12">
+        <v>104.502647181491</v>
+      </c>
+      <c r="N5" s="12">
+        <v>222.474010803976</v>
+      </c>
+      <c r="O5" s="12">
+        <v>222.474010803976</v>
+      </c>
+      <c r="P5" s="12">
+        <v>222.474010803976</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>386.69704673303698</v>
+      </c>
+      <c r="R5" s="17">
+        <v>386.69704673303698</v>
+      </c>
+      <c r="S5" s="17">
+        <v>386.69704673303698</v>
+      </c>
+      <c r="T5" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U5" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V5" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W5" s="12">
+        <v>184.30516162050699</v>
+      </c>
+      <c r="X5" s="12">
+        <v>184.30516162050699</v>
+      </c>
+      <c r="Y5" s="12">
+        <v>184.30516162050699</v>
+      </c>
+      <c r="Z5" s="12">
+        <v>267.28971360777098</v>
+      </c>
+      <c r="AA5" s="12">
+        <v>267.28971360777098</v>
+      </c>
+      <c r="AB5" s="12">
+        <v>267.28971360777098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="9">
         <v>109.06640537006101</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
         <v>371.10373938623502</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
         <v>656.92524278001895</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="12">
+        <v>112.126988612815</v>
+      </c>
+      <c r="L6" s="12">
+        <v>112.126988612815</v>
+      </c>
+      <c r="M6" s="12">
+        <v>112.126988612815</v>
+      </c>
+      <c r="N6" s="12">
+        <v>253.62405427708501</v>
+      </c>
+      <c r="O6" s="12">
+        <v>253.62405427708501</v>
+      </c>
+      <c r="P6" s="12">
+        <v>253.62405427708501</v>
+      </c>
+      <c r="Q6" s="17">
+        <v>383.01045494758699</v>
+      </c>
+      <c r="R6" s="17">
+        <v>383.01045494758699</v>
+      </c>
+      <c r="S6" s="17">
+        <v>383.01045494758699</v>
+      </c>
+      <c r="T6" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U6" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V6" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W6" s="12">
+        <v>186.15034094391899</v>
+      </c>
+      <c r="X6" s="12">
+        <v>186.15034094391899</v>
+      </c>
+      <c r="Y6" s="12">
+        <v>186.15034094391899</v>
+      </c>
+      <c r="Z6" s="12">
+        <v>294.26728457041298</v>
+      </c>
+      <c r="AA6" s="12">
+        <v>294.26728457041298</v>
+      </c>
+      <c r="AB6" s="12">
+        <v>294.26728457041298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="9">
         <v>114.672527883984</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
         <v>335.99770274310202</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
         <v>650.18255249745698</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="L7" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="M7" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="N7" s="12">
+        <v>233.61735718372</v>
+      </c>
+      <c r="O7" s="12">
+        <v>233.61735718372</v>
+      </c>
+      <c r="P7" s="12">
+        <v>233.61735718372</v>
+      </c>
+      <c r="Q7" s="17">
+        <v>379.68459871468798</v>
+      </c>
+      <c r="R7" s="17">
+        <v>379.68459871468798</v>
+      </c>
+      <c r="S7" s="17">
+        <v>379.68459871468798</v>
+      </c>
+      <c r="T7" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="U7" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="V7" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="W7" s="12">
+        <v>183.157645322219</v>
+      </c>
+      <c r="X7" s="12">
+        <v>183.157645322219</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>183.157645322219</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>288.18248751780999</v>
+      </c>
+      <c r="AA7" s="12">
+        <v>288.18248751780999</v>
+      </c>
+      <c r="AB7" s="12">
+        <v>288.18248751780999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="9">
         <v>110.714297590952</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <v>350.06659003440097</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>708.91130290037995</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="12">
+        <v>105.412720908233</v>
+      </c>
+      <c r="L8" s="12">
+        <v>105.412720908233</v>
+      </c>
+      <c r="M8" s="12">
+        <v>105.412720908233</v>
+      </c>
+      <c r="N8" s="12">
+        <v>243.639587743362</v>
+      </c>
+      <c r="O8" s="12">
+        <v>243.639587743362</v>
+      </c>
+      <c r="P8" s="12">
+        <v>243.639587743362</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>383.48539681657797</v>
+      </c>
+      <c r="R8" s="17">
+        <v>383.48539681657797</v>
+      </c>
+      <c r="S8" s="17">
+        <v>383.48539681657797</v>
+      </c>
+      <c r="T8" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U8" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V8" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W8" s="12">
+        <v>183.53375580801301</v>
+      </c>
+      <c r="X8" s="12">
+        <v>183.53375580801301</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>183.53375580801301</v>
+      </c>
+      <c r="Z8" s="12">
+        <v>288.54385933297101</v>
+      </c>
+      <c r="AA8" s="12">
+        <v>288.54385933297101</v>
+      </c>
+      <c r="AB8" s="12">
+        <v>288.54385933297101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="9">
         <v>112.13063098420101</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
         <v>362.67308829763198</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9">
         <v>677.21232598429197</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="12">
+        <v>99.200383060045596</v>
+      </c>
+      <c r="L9" s="12">
+        <v>99.200383060045596</v>
+      </c>
+      <c r="M9" s="12">
+        <v>99.200383060045596</v>
+      </c>
+      <c r="N9" s="12">
+        <v>242.93297365162999</v>
+      </c>
+      <c r="O9" s="12">
+        <v>242.93297365162999</v>
+      </c>
+      <c r="P9" s="12">
+        <v>242.93297365162999</v>
+      </c>
+      <c r="Q9" s="17">
+        <v>389.51361128194401</v>
+      </c>
+      <c r="R9" s="17">
+        <v>389.51361128194401</v>
+      </c>
+      <c r="S9" s="17">
+        <v>389.51361128194401</v>
+      </c>
+      <c r="T9" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="U9" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="V9" s="12">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="W9" s="12">
+        <v>179.948493600825</v>
+      </c>
+      <c r="X9" s="12">
+        <v>179.948493600825</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>179.948493600825</v>
+      </c>
+      <c r="Z9" s="12">
+        <v>287.97083681570399</v>
+      </c>
+      <c r="AA9" s="12">
+        <v>287.97083681570399</v>
+      </c>
+      <c r="AB9" s="12">
+        <v>287.97083681570399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="9">
         <v>96.9600276990992</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
         <v>352.835788325392</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>643.08320144635002</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="L10" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="M10" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="N10" s="12">
+        <v>257.97167897401602</v>
+      </c>
+      <c r="O10" s="12">
+        <v>257.97167897401602</v>
+      </c>
+      <c r="P10" s="12">
+        <v>257.97167897401602</v>
+      </c>
+      <c r="Q10" s="17">
+        <v>388.86594001400402</v>
+      </c>
+      <c r="R10" s="17">
+        <v>388.86594001400402</v>
+      </c>
+      <c r="S10" s="17">
+        <v>388.86594001400402</v>
+      </c>
+      <c r="T10" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U10" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V10" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W10" s="12">
+        <v>188.46713750415799</v>
+      </c>
+      <c r="X10" s="12">
+        <v>188.46713750415799</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>188.46713750415799</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>287.96479689935899</v>
+      </c>
+      <c r="AA10" s="12">
+        <v>287.96479689935899</v>
+      </c>
+      <c r="AB10" s="12">
+        <v>287.96479689935899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="16">
         <v>101.00962122129</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="9">
         <v>361.35473004270398</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9">
         <v>644.79579278079495</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="L11" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="M11" s="12">
+        <v>108.702547057549</v>
+      </c>
+      <c r="N11" s="12">
+        <v>240.577093504836</v>
+      </c>
+      <c r="O11" s="12">
+        <v>240.577093504836</v>
+      </c>
+      <c r="P11" s="12">
+        <v>240.577093504836</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>384.781070870257</v>
+      </c>
+      <c r="R11" s="17">
+        <v>384.781070870257</v>
+      </c>
+      <c r="S11" s="17">
+        <v>384.781070870257</v>
+      </c>
+      <c r="T11" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U11" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V11" s="12">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W11" s="12">
+        <v>184.864937609213</v>
+      </c>
+      <c r="X11" s="12">
+        <v>184.864937609213</v>
+      </c>
+      <c r="Y11" s="12">
+        <v>184.864937609213</v>
+      </c>
+      <c r="Z11" s="12">
+        <v>277.95627447967303</v>
+      </c>
+      <c r="AA11" s="12">
+        <v>277.95627447967303</v>
+      </c>
+      <c r="AB11" s="12">
+        <v>277.95627447967303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="10">
         <v>111.37281536988201</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10">
         <v>332.21439008042501</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10">
         <v>664.94307721541202</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="18">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="L12" s="18">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="M12" s="18">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="N12" s="18">
+        <v>235.665599379154</v>
+      </c>
+      <c r="O12" s="18">
+        <v>235.665599379154</v>
+      </c>
+      <c r="P12" s="18">
+        <v>235.665599379154</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>384.322192043661</v>
+      </c>
+      <c r="R12" s="19">
+        <v>384.322192043661</v>
+      </c>
+      <c r="S12" s="19">
+        <v>384.322192043661</v>
+      </c>
+      <c r="T12" s="20">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U12" s="20">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V12" s="20">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W12" s="20">
+        <v>184.492488729847</v>
+      </c>
+      <c r="X12" s="20">
+        <v>184.492488729847</v>
+      </c>
+      <c r="Y12" s="20">
+        <v>184.492488729847</v>
+      </c>
+      <c r="Z12" s="20">
+        <v>281.14025661968702</v>
+      </c>
+      <c r="AA12" s="20">
+        <v>281.14025661968702</v>
+      </c>
+      <c r="AB12" s="20">
+        <v>281.14025661968702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="8">
         <v>107.76192819246501</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="8">
         <v>349.41023261461902</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
       <c r="H13" s="8">
         <v>663.65498725129999</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8">
+        <f>AVERAGE(K3:M12)</f>
+        <v>104.84573521623409</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8">
+        <f>AVERAGE(N3:P12)</f>
+        <v>242.33829198431738</v>
+      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8">
+        <f>AVERAGE(Q3:S12)</f>
+        <v>383.84999799029907</v>
+      </c>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8">
+        <f>AVERAGE(T3:V12)</f>
+        <v>96.097444769616544</v>
+      </c>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8">
+        <f>AVERAGE(W3:Y12)</f>
+        <v>183.70921710830464</v>
+      </c>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8">
+        <f>AVERAGE(Z3:AB12)</f>
+        <v>286.44229044720799</v>
+      </c>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="8">
         <v>5.6392991317875802</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="8">
         <v>12.142768009877701</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="8">
         <v>18.9268913224439</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8">
+        <f>_xlfn.STDEV.P(K3:M12)</f>
+        <v>5.4244521265497978</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8">
+        <f>_xlfn.STDEV.P(N3:P12)</f>
+        <v>9.6933247093149379</v>
+      </c>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8">
+        <f>_xlfn.STDEV.P(Q3:S12)</f>
+        <v>6.3168514486314642</v>
+      </c>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8">
+        <f>_xlfn.STDEV.P(T3:V12)</f>
+        <v>6.8586307442042665E-2</v>
+      </c>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8">
+        <f>_xlfn.STDEV.P(W3:Y12)</f>
+        <v>2.8023197675971754</v>
+      </c>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8">
+        <f>_xlfn.STDEV.P(Z3:AB12)</f>
+        <v>8.6242133995334544</v>
+      </c>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="7">
         <v>103.509601217861</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="7">
         <v>112.014255167069</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="7">
         <v>340.25394940493601</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="7">
         <v>358.56651582430101</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="7">
         <v>649.38311966013805</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="7">
         <v>677.92685484246203</v>
       </c>
+      <c r="K15" s="7">
+        <v>100.96558551755066</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="7">
+        <v>108.72588491491751</v>
+      </c>
+      <c r="N15" s="7">
+        <f t="shared" ref="N15" si="0">N7-N14</f>
+        <v>223.92403247440507</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15" s="7">
+        <f t="shared" ref="P15" si="1">P6+P13</f>
+        <v>253.62405427708501</v>
+      </c>
+      <c r="Q15" s="7">
+        <f t="shared" ref="Q15" si="2">Q7-Q14</f>
+        <v>373.36774726605654</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="S15" s="7">
+        <f t="shared" ref="S15" si="3">S6+S13</f>
+        <v>383.01045494758699</v>
+      </c>
+      <c r="T15" s="7">
+        <v>96.048384489620247</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="V15" s="7">
+        <v>96.146505049612841</v>
+      </c>
+      <c r="W15" s="7">
+        <v>181.7046975829802</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y15" s="7">
+        <v>185.71373663362908</v>
+      </c>
+      <c r="Z15" s="7">
+        <v>280.27332845014354</v>
+      </c>
+      <c r="AA15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB15" s="7">
+        <v>292.61125244427245</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="E25" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="120">
+    <mergeCell ref="W14:Y14"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="Z6:AB6"/>
+    <mergeCell ref="Z7:AB7"/>
+    <mergeCell ref="Z8:AB8"/>
+    <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="Z10:AB10"/>
+    <mergeCell ref="Z11:AB11"/>
+    <mergeCell ref="Z12:AB12"/>
+    <mergeCell ref="Z13:AB13"/>
+    <mergeCell ref="Z14:AB14"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="W6:Y6"/>
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="W8:Y8"/>
+    <mergeCell ref="W9:Y9"/>
+    <mergeCell ref="W10:Y10"/>
+    <mergeCell ref="W11:Y11"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="W13:Y13"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="T1:AB1"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="H14:J14"/>
@@ -836,34 +1730,7 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adaugat testul Wilcoxon pentru semn
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azza/Workspace/FAC/SEM 3/AEA/aea_tsp_with_drone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBDD8CD-AB07-234B-8757-119132DCAEAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5170C70-7B17-6440-AF01-B21A71009A96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>AG</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>ACO OPTIMIZAT</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Wcrit</t>
+  </si>
+  <si>
+    <t>Wcrit one tail</t>
+  </si>
+  <si>
+    <t>Se respinge ipoteza nula</t>
+  </si>
+  <si>
+    <t>Wilcoxon test AG VS ACO</t>
+  </si>
+  <si>
+    <t>Wilcoxon test AG VS ACO optimizat</t>
   </si>
 </sst>
 </file>
@@ -214,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,14 +249,41 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,32 +291,14 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:AB1"/>
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -565,166 +592,168 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.33203125" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
     <col min="12" max="12" width="4" customWidth="1"/>
-    <col min="15" max="15" width="4.1640625" customWidth="1"/>
+    <col min="13" max="13" width="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="21" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="18" t="s">
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="15" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="16" t="s">
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="17" t="s">
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="15" t="s">
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="17" t="s">
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="17">
         <v>112.298255214972</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17">
         <v>336.36589344233101</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17">
         <v>651.31643783594097</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="13">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="10">
         <v>249.07310752944301</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="10">
         <v>249.07310752944301</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="10">
         <v>249.07310752944301</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="10">
         <v>390.66091126679902</v>
       </c>
-      <c r="R3" s="13">
+      <c r="R3" s="10">
         <v>390.66091126679902</v>
       </c>
-      <c r="S3" s="13">
+      <c r="S3" s="10">
         <v>390.66091126679902</v>
       </c>
-      <c r="T3" s="13">
+      <c r="T3" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="U3" s="13">
+      <c r="U3" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="V3" s="13">
+      <c r="V3" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="W3" s="13">
+      <c r="W3" s="10">
         <v>177.97248805664199</v>
       </c>
-      <c r="X3" s="13">
+      <c r="X3" s="10">
         <v>177.97248805664199</v>
       </c>
-      <c r="Y3" s="13">
+      <c r="Y3" s="10">
         <v>177.97248805664199</v>
       </c>
-      <c r="Z3" s="13">
+      <c r="Z3" s="10">
         <v>299.88151301964501</v>
       </c>
-      <c r="AA3" s="13">
+      <c r="AA3" s="10">
         <v>299.88151301964501</v>
       </c>
-      <c r="AB3" s="13">
+      <c r="AB3" s="10">
         <v>299.88151301964501</v>
       </c>
     </row>
@@ -732,73 +761,73 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="17">
         <v>101.086110834465</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17">
         <v>346.24902424644199</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17">
         <v>661.83348648440199</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="13">
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="10">
         <v>243.80745679595199</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="10">
         <v>243.80745679595199</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="10">
         <v>243.80745679595199</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="10">
         <v>367.478757214437</v>
       </c>
-      <c r="R4" s="13">
+      <c r="R4" s="10">
         <v>367.478757214437</v>
       </c>
-      <c r="S4" s="13">
+      <c r="S4" s="10">
         <v>367.478757214437</v>
       </c>
-      <c r="T4" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="U4" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="V4" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="W4" s="13">
+      <c r="T4" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U4" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V4" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W4" s="10">
         <v>184.19972188770399</v>
       </c>
-      <c r="X4" s="13">
+      <c r="X4" s="10">
         <v>184.19972188770399</v>
       </c>
-      <c r="Y4" s="13">
+      <c r="Y4" s="10">
         <v>184.19972188770399</v>
       </c>
-      <c r="Z4" s="13">
+      <c r="Z4" s="10">
         <v>291.22588160904797</v>
       </c>
-      <c r="AA4" s="13">
+      <c r="AA4" s="10">
         <v>291.22588160904797</v>
       </c>
-      <c r="AB4" s="13">
+      <c r="AB4" s="10">
         <v>291.22588160904797</v>
       </c>
     </row>
@@ -806,73 +835,73 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="17">
         <v>108.30858975574201</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17">
         <v>345.24137954752302</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17">
         <v>677.34645258795103</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="13">
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="10">
         <v>104.502647181491</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="10">
         <v>104.502647181491</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="10">
         <v>104.502647181491</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="10">
         <v>222.474010803976</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="10">
         <v>222.474010803976</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="10">
         <v>222.474010803976</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="10">
         <v>386.69704673303698</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="10">
         <v>386.69704673303698</v>
       </c>
-      <c r="S5" s="13">
+      <c r="S5" s="10">
         <v>386.69704673303698</v>
       </c>
-      <c r="T5" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="U5" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="V5" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="W5" s="13">
+      <c r="T5" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U5" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V5" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W5" s="10">
         <v>184.30516162050699</v>
       </c>
-      <c r="X5" s="13">
+      <c r="X5" s="10">
         <v>184.30516162050699</v>
       </c>
-      <c r="Y5" s="13">
+      <c r="Y5" s="10">
         <v>184.30516162050699</v>
       </c>
-      <c r="Z5" s="13">
+      <c r="Z5" s="10">
         <v>267.28971360777098</v>
       </c>
-      <c r="AA5" s="13">
+      <c r="AA5" s="10">
         <v>267.28971360777098</v>
       </c>
-      <c r="AB5" s="13">
+      <c r="AB5" s="10">
         <v>267.28971360777098</v>
       </c>
     </row>
@@ -880,73 +909,73 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="17">
         <v>109.06640537006101</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17">
         <v>371.10373938623502</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17">
         <v>656.92524278001895</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="13">
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="10">
         <v>112.126988612815</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="10">
         <v>112.126988612815</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="10">
         <v>112.126988612815</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="10">
         <v>253.62405427708501</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="10">
         <v>253.62405427708501</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="10">
         <v>253.62405427708501</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="10">
         <v>383.01045494758699</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="10">
         <v>383.01045494758699</v>
       </c>
-      <c r="S6" s="13">
+      <c r="S6" s="10">
         <v>383.01045494758699</v>
       </c>
-      <c r="T6" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="U6" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="V6" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="W6" s="13">
+      <c r="T6" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U6" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V6" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W6" s="10">
         <v>186.15034094391899</v>
       </c>
-      <c r="X6" s="13">
+      <c r="X6" s="10">
         <v>186.15034094391899</v>
       </c>
-      <c r="Y6" s="13">
+      <c r="Y6" s="10">
         <v>186.15034094391899</v>
       </c>
-      <c r="Z6" s="13">
+      <c r="Z6" s="10">
         <v>294.26728457041298</v>
       </c>
-      <c r="AA6" s="13">
+      <c r="AA6" s="10">
         <v>294.26728457041298</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AB6" s="10">
         <v>294.26728457041298</v>
       </c>
     </row>
@@ -954,73 +983,73 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="17">
         <v>114.672527883984</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17">
         <v>335.99770274310202</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17">
         <v>650.18255249745698</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="13">
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="10">
         <v>233.61735718372</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="10">
         <v>233.61735718372</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="10">
         <v>233.61735718372</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="10">
         <v>379.68459871468798</v>
       </c>
-      <c r="R7" s="13">
+      <c r="R7" s="10">
         <v>379.68459871468798</v>
       </c>
-      <c r="S7" s="13">
+      <c r="S7" s="10">
         <v>379.68459871468798</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="U7" s="13">
+      <c r="U7" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="V7" s="13">
+      <c r="V7" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="W7" s="13">
+      <c r="W7" s="10">
         <v>183.157645322219</v>
       </c>
-      <c r="X7" s="13">
+      <c r="X7" s="10">
         <v>183.157645322219</v>
       </c>
-      <c r="Y7" s="13">
+      <c r="Y7" s="10">
         <v>183.157645322219</v>
       </c>
-      <c r="Z7" s="13">
+      <c r="Z7" s="10">
         <v>288.18248751780999</v>
       </c>
-      <c r="AA7" s="13">
+      <c r="AA7" s="10">
         <v>288.18248751780999</v>
       </c>
-      <c r="AB7" s="13">
+      <c r="AB7" s="10">
         <v>288.18248751780999</v>
       </c>
     </row>
@@ -1028,73 +1057,73 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="17">
         <v>110.714297590952</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17">
         <v>350.06659003440097</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17">
         <v>708.91130290037995</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="13">
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="10">
         <v>105.412720908233</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="10">
         <v>105.412720908233</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="10">
         <v>105.412720908233</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="10">
         <v>243.639587743362</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="10">
         <v>243.639587743362</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="10">
         <v>243.639587743362</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="10">
         <v>383.48539681657797</v>
       </c>
-      <c r="R8" s="13">
+      <c r="R8" s="10">
         <v>383.48539681657797</v>
       </c>
-      <c r="S8" s="13">
+      <c r="S8" s="10">
         <v>383.48539681657797</v>
       </c>
-      <c r="T8" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="U8" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="V8" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="W8" s="13">
+      <c r="T8" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U8" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V8" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W8" s="10">
         <v>183.53375580801301</v>
       </c>
-      <c r="X8" s="13">
+      <c r="X8" s="10">
         <v>183.53375580801301</v>
       </c>
-      <c r="Y8" s="13">
+      <c r="Y8" s="10">
         <v>183.53375580801301</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="Z8" s="10">
         <v>288.54385933297101</v>
       </c>
-      <c r="AA8" s="13">
+      <c r="AA8" s="10">
         <v>288.54385933297101</v>
       </c>
-      <c r="AB8" s="13">
+      <c r="AB8" s="10">
         <v>288.54385933297101</v>
       </c>
     </row>
@@ -1102,73 +1131,73 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="17">
         <v>112.13063098420101</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17">
         <v>362.67308829763198</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17">
         <v>677.21232598429197</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="13">
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="10">
         <v>99.200383060045596</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="10">
         <v>99.200383060045596</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="10">
         <v>99.200383060045596</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="10">
         <v>242.93297365162999</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="10">
         <v>242.93297365162999</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="10">
         <v>242.93297365162999</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="10">
         <v>389.51361128194401</v>
       </c>
-      <c r="R9" s="13">
+      <c r="R9" s="10">
         <v>389.51361128194401</v>
       </c>
-      <c r="S9" s="13">
+      <c r="S9" s="10">
         <v>389.51361128194401</v>
       </c>
-      <c r="T9" s="13">
+      <c r="T9" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="U9" s="13">
+      <c r="U9" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="V9" s="13">
+      <c r="V9" s="10">
         <v>96.202212084780101</v>
       </c>
-      <c r="W9" s="13">
+      <c r="W9" s="10">
         <v>179.948493600825</v>
       </c>
-      <c r="X9" s="13">
+      <c r="X9" s="10">
         <v>179.948493600825</v>
       </c>
-      <c r="Y9" s="13">
+      <c r="Y9" s="10">
         <v>179.948493600825</v>
       </c>
-      <c r="Z9" s="13">
+      <c r="Z9" s="10">
         <v>287.97083681570399</v>
       </c>
-      <c r="AA9" s="13">
+      <c r="AA9" s="10">
         <v>287.97083681570399</v>
       </c>
-      <c r="AB9" s="13">
+      <c r="AB9" s="10">
         <v>287.97083681570399</v>
       </c>
     </row>
@@ -1176,73 +1205,73 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="17">
         <v>96.9600276990992</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17">
         <v>352.835788325392</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17">
         <v>643.08320144635002</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="13">
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="10">
         <v>257.97167897401602</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="10">
         <v>257.97167897401602</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P10" s="10">
         <v>257.97167897401602</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="10">
         <v>388.86594001400402</v>
       </c>
-      <c r="R10" s="13">
+      <c r="R10" s="10">
         <v>388.86594001400402</v>
       </c>
-      <c r="S10" s="13">
+      <c r="S10" s="10">
         <v>388.86594001400402</v>
       </c>
-      <c r="T10" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="U10" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="V10" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="W10" s="13">
+      <c r="T10" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U10" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V10" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W10" s="10">
         <v>188.46713750415799</v>
       </c>
-      <c r="X10" s="13">
+      <c r="X10" s="10">
         <v>188.46713750415799</v>
       </c>
-      <c r="Y10" s="13">
+      <c r="Y10" s="10">
         <v>188.46713750415799</v>
       </c>
-      <c r="Z10" s="13">
+      <c r="Z10" s="10">
         <v>287.96479689935899</v>
       </c>
-      <c r="AA10" s="13">
+      <c r="AA10" s="10">
         <v>287.96479689935899</v>
       </c>
-      <c r="AB10" s="13">
+      <c r="AB10" s="10">
         <v>287.96479689935899</v>
       </c>
     </row>
@@ -1250,73 +1279,73 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="21">
         <v>101.00962122129</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="10">
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="17">
         <v>361.35473004270398</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10">
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17">
         <v>644.79579278079495</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="13">
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="10">
         <v>108.702547057549</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="10">
         <v>240.577093504836</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="10">
         <v>240.577093504836</v>
       </c>
-      <c r="P11" s="13">
+      <c r="P11" s="10">
         <v>240.577093504836</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="Q11" s="10">
         <v>384.781070870257</v>
       </c>
-      <c r="R11" s="13">
+      <c r="R11" s="10">
         <v>384.781070870257</v>
       </c>
-      <c r="S11" s="13">
+      <c r="S11" s="10">
         <v>384.781070870257</v>
       </c>
-      <c r="T11" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="U11" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="V11" s="13">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="W11" s="13">
+      <c r="T11" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U11" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V11" s="10">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W11" s="10">
         <v>184.864937609213</v>
       </c>
-      <c r="X11" s="13">
+      <c r="X11" s="10">
         <v>184.864937609213</v>
       </c>
-      <c r="Y11" s="13">
+      <c r="Y11" s="10">
         <v>184.864937609213</v>
       </c>
-      <c r="Z11" s="13">
+      <c r="Z11" s="10">
         <v>277.95627447967303</v>
       </c>
-      <c r="AA11" s="13">
+      <c r="AA11" s="10">
         <v>277.95627447967303</v>
       </c>
-      <c r="AB11" s="13">
+      <c r="AB11" s="10">
         <v>277.95627447967303</v>
       </c>
     </row>
@@ -1324,73 +1353,73 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="20">
         <v>111.37281536988201</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20">
         <v>332.21439008042501</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11">
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20">
         <v>664.94307721541202</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="19">
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="14">
         <v>96.202212084780101</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L12" s="14">
         <v>96.202212084780101</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="14">
         <v>96.202212084780101</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="14">
         <v>235.665599379154</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="14">
         <v>235.665599379154</v>
       </c>
-      <c r="P12" s="19">
+      <c r="P12" s="14">
         <v>235.665599379154</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q12" s="14">
         <v>384.322192043661</v>
       </c>
-      <c r="R12" s="19">
+      <c r="R12" s="14">
         <v>384.322192043661</v>
       </c>
-      <c r="S12" s="19">
+      <c r="S12" s="14">
         <v>384.322192043661</v>
       </c>
-      <c r="T12" s="20">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="U12" s="20">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="V12" s="20">
-        <v>96.052544491689304</v>
-      </c>
-      <c r="W12" s="20">
+      <c r="T12" s="11">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="U12" s="11">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="V12" s="11">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="W12" s="11">
         <v>184.492488729847</v>
       </c>
-      <c r="X12" s="20">
+      <c r="X12" s="11">
         <v>184.492488729847</v>
       </c>
-      <c r="Y12" s="20">
+      <c r="Y12" s="11">
         <v>184.492488729847</v>
       </c>
-      <c r="Z12" s="20">
+      <c r="Z12" s="11">
         <v>281.14025661968702</v>
       </c>
-      <c r="AA12" s="20">
+      <c r="AA12" s="11">
         <v>281.14025661968702</v>
       </c>
-      <c r="AB12" s="20">
+      <c r="AB12" s="11">
         <v>281.14025661968702</v>
       </c>
     </row>
@@ -1398,113 +1427,113 @@
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>107.76192819246501</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8">
         <v>349.41023261461902</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8">
         <v>663.65498725129999</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9">
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8">
         <f>AVERAGE(K3:M12)</f>
         <v>104.84573521623409</v>
       </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9">
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8">
         <f>AVERAGE(N3:P12)</f>
         <v>242.33829198431738</v>
       </c>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9">
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8">
         <f>AVERAGE(Q3:S12)</f>
         <v>383.84999799029907</v>
       </c>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9">
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8">
         <f>AVERAGE(T3:V12)</f>
         <v>96.097444769616544</v>
       </c>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9">
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8">
         <f>AVERAGE(W3:Y12)</f>
         <v>183.70921710830464</v>
       </c>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9">
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8">
         <f>AVERAGE(Z3:AB12)</f>
         <v>286.44229044720799</v>
       </c>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>5.6392991317875802</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8">
         <v>12.142768009877701</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8">
         <v>18.9268913224439</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9">
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8">
         <f>_xlfn.STDEV.P(K3:M12)</f>
         <v>5.4244521265497978</v>
       </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9">
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8">
         <f>_xlfn.STDEV.P(N3:P12)</f>
         <v>9.6933247093149379</v>
       </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9">
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8">
         <f>_xlfn.STDEV.P(Q3:S12)</f>
         <v>6.3168514486314642</v>
       </c>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9">
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8">
         <f>_xlfn.STDEV.P(T3:V12)</f>
         <v>6.8586307442042665E-2</v>
       </c>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9">
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8">
         <f>_xlfn.STDEV.P(W3:Y12)</f>
         <v>2.8023197675971754</v>
       </c>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9">
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8">
         <f>_xlfn.STDEV.P(Z3:AB12)</f>
         <v>8.6242133995334544</v>
       </c>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -1597,17 +1626,17 @@
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:31" x14ac:dyDescent="0.2">
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1618,7 +1647,7 @@
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:31" x14ac:dyDescent="0.2">
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1629,11 +1658,650 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.2">
       <c r="E25" s="6"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="D27" s="23">
+        <v>109.06640537006101</v>
+      </c>
+      <c r="E27" s="23">
+        <v>112.126988612815</v>
+      </c>
+      <c r="F27" s="23">
+        <f>ABS(D27-E27)</f>
+        <v>3.0605832427539923</v>
+      </c>
+      <c r="G27">
+        <f>SIGN(D27-E27)</f>
+        <v>-1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f>G27*H27</f>
+        <v>-1</v>
+      </c>
+      <c r="M27" s="23">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="N27" s="2">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="O27" s="23">
+        <f>ABS(M27-N27)</f>
+        <v>0.14966759309079691</v>
+      </c>
+      <c r="P27">
+        <f>SIGN(M27-N27)</f>
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <f>P27*Q27</f>
+        <v>1</v>
+      </c>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="D28" s="22">
+        <v>112.298255214972</v>
+      </c>
+      <c r="E28" s="22">
+        <v>108.702547057549</v>
+      </c>
+      <c r="F28" s="23">
+        <f>ABS(D28-E28)</f>
+        <v>3.5957081574230045</v>
+      </c>
+      <c r="G28">
+        <f>SIGN(D28-E28)</f>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <f t="shared" ref="I28:I36" si="4">G28*H28</f>
+        <v>2</v>
+      </c>
+      <c r="M28" s="22">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="N28" s="2">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="O28" s="23">
+        <f>ABS(M28-N28)</f>
+        <v>0.14966759309079691</v>
+      </c>
+      <c r="P28">
+        <f>SIGN(M28-N28)</f>
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>2</v>
+      </c>
+      <c r="R28">
+        <f>P28*Q28</f>
+        <v>2</v>
+      </c>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="D29" s="23">
+        <v>108.30858975574201</v>
+      </c>
+      <c r="E29" s="23">
+        <v>104.502647181491</v>
+      </c>
+      <c r="F29" s="23">
+        <f>ABS(D29-E29)</f>
+        <v>3.8059425742510058</v>
+      </c>
+      <c r="G29">
+        <f>SIGN(D29-E29)</f>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M29" s="22">
+        <v>99.200383060045596</v>
+      </c>
+      <c r="N29" s="2">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="O29" s="23">
+        <f>ABS(M29-N29)</f>
+        <v>3.1478385683562919</v>
+      </c>
+      <c r="P29">
+        <f>SIGN(M29-N29)</f>
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>3</v>
+      </c>
+      <c r="R29">
+        <f>P29*Q29</f>
+        <v>3</v>
+      </c>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="D30" s="23">
+        <v>101.086110834465</v>
+      </c>
+      <c r="E30" s="23">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="F30" s="23">
+        <f>ABS(D30-E30)</f>
+        <v>4.8838987496849029</v>
+      </c>
+      <c r="G30">
+        <f>SIGN(D30-E30)</f>
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="M30" s="23">
+        <v>104.502647181491</v>
+      </c>
+      <c r="N30" s="2">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="O30" s="23">
+        <f>ABS(M30-N30)</f>
+        <v>8.450102689801696</v>
+      </c>
+      <c r="P30">
+        <f>SIGN(M30-N30)</f>
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>4</v>
+      </c>
+      <c r="R30">
+        <f>P30*Q30</f>
+        <v>4</v>
+      </c>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="D31" s="23">
+        <v>110.714297590952</v>
+      </c>
+      <c r="E31" s="23">
+        <v>105.412720908233</v>
+      </c>
+      <c r="F31" s="23">
+        <f>ABS(D31-E31)</f>
+        <v>5.3015766827190021</v>
+      </c>
+      <c r="G31">
+        <f>SIGN(D31-E31)</f>
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="M31" s="23">
+        <v>105.412720908233</v>
+      </c>
+      <c r="N31" s="2">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="O31" s="23">
+        <f>ABS(M31-N31)</f>
+        <v>9.2105088234528978</v>
+      </c>
+      <c r="P31">
+        <f>SIGN(M31-N31)</f>
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>5</v>
+      </c>
+      <c r="R31">
+        <f>P31*Q31</f>
+        <v>5</v>
+      </c>
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="D32" s="23">
+        <v>114.672527883984</v>
+      </c>
+      <c r="E32" s="23">
+        <v>108.702547057549</v>
+      </c>
+      <c r="F32" s="23">
+        <f>ABS(D32-E32)</f>
+        <v>5.9699808264350054</v>
+      </c>
+      <c r="G32">
+        <f>SIGN(D32-E32)</f>
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>6</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="M32" s="22">
+        <v>108.702547057549</v>
+      </c>
+      <c r="N32" s="2">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="O32" s="23">
+        <f>ABS(M32-N32)</f>
+        <v>12.500334972768897</v>
+      </c>
+      <c r="P32">
+        <f>SIGN(M32-N32)</f>
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>6</v>
+      </c>
+      <c r="R32">
+        <f>P32*Q32</f>
+        <v>6</v>
+      </c>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D33" s="22">
+        <v>101.00962122129</v>
+      </c>
+      <c r="E33" s="22">
+        <v>108.702547057549</v>
+      </c>
+      <c r="F33" s="23">
+        <f>ABS(D33-E33)</f>
+        <v>7.6929258362589934</v>
+      </c>
+      <c r="G33">
+        <f>SIGN(D33-E33)</f>
+        <v>-1</v>
+      </c>
+      <c r="H33">
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="4"/>
+        <v>-7</v>
+      </c>
+      <c r="M33" s="22">
+        <v>108.702547057549</v>
+      </c>
+      <c r="N33" s="2">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="O33" s="23">
+        <f>ABS(M33-N33)</f>
+        <v>12.650002565859694</v>
+      </c>
+      <c r="P33">
+        <f>SIGN(M33-N33)</f>
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>7</v>
+      </c>
+      <c r="R33">
+        <f>P33*Q33</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D34" s="23">
+        <v>96.9600276990992</v>
+      </c>
+      <c r="E34" s="23">
+        <v>108.702547057549</v>
+      </c>
+      <c r="F34" s="23">
+        <f>ABS(D34-E34)</f>
+        <v>11.742519358449798</v>
+      </c>
+      <c r="G34">
+        <f>SIGN(D34-E34)</f>
+        <v>-1</v>
+      </c>
+      <c r="H34">
+        <v>8</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="4"/>
+        <v>-8</v>
+      </c>
+      <c r="M34" s="23">
+        <v>108.702547057549</v>
+      </c>
+      <c r="N34" s="2">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="O34" s="23">
+        <f>ABS(M34-N34)</f>
+        <v>12.650002565859694</v>
+      </c>
+      <c r="P34">
+        <f>SIGN(M34-N34)</f>
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>8</v>
+      </c>
+      <c r="R34">
+        <f>P34*Q34</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D35" s="24">
+        <v>112.13063098420101</v>
+      </c>
+      <c r="E35" s="24">
+        <v>99.200383060045596</v>
+      </c>
+      <c r="F35" s="23">
+        <f>ABS(D35-E35)</f>
+        <v>12.93024792415541</v>
+      </c>
+      <c r="G35">
+        <f>SIGN(D35-E35)</f>
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>9</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="M35" s="23">
+        <v>108.702547057549</v>
+      </c>
+      <c r="N35" s="2">
+        <v>96.052544491689304</v>
+      </c>
+      <c r="O35" s="23">
+        <f>ABS(M35-N35)</f>
+        <v>12.650002565859694</v>
+      </c>
+      <c r="P35">
+        <f>SIGN(M35-N35)</f>
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>9</v>
+      </c>
+      <c r="R35">
+        <f>P35*Q35</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D36" s="22">
+        <v>111.37281536988201</v>
+      </c>
+      <c r="E36" s="22">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="F36" s="23">
+        <f>ABS(D36-E36)</f>
+        <v>15.170603285101905</v>
+      </c>
+      <c r="G36">
+        <f>SIGN(D36-E36)</f>
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>10</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="M36" s="24">
+        <v>112.126988612815</v>
+      </c>
+      <c r="N36" s="2">
+        <v>96.202212084780101</v>
+      </c>
+      <c r="O36" s="23">
+        <f>ABS(M36-N36)</f>
+        <v>15.924776528034897</v>
+      </c>
+      <c r="P36">
+        <f>SIGN(M36-N36)</f>
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>10</v>
+      </c>
+      <c r="R36">
+        <f>P36*Q36</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37">
+        <f>ABS(SUM(I27:I36))</f>
+        <v>23</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>10</v>
+      </c>
+      <c r="R37">
+        <f>ABS(SUM(R28:R36))</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>11</v>
+      </c>
+      <c r="R38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39">
+        <v>10</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>12</v>
+      </c>
+      <c r="R39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="M26:R40">
+    <sortCondition ref="O27"/>
+  </sortState>
   <mergeCells count="121">
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="T1:AB1"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="W4:Y4"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="W6:Y6"/>
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="W8:Y8"/>
     <mergeCell ref="W14:Y14"/>
     <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="Z3:AB3"/>
@@ -1653,108 +2321,6 @@
     <mergeCell ref="W11:Y11"/>
     <mergeCell ref="W12:Y12"/>
     <mergeCell ref="W13:Y13"/>
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="T10:V10"/>
-    <mergeCell ref="T1:AB1"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="W4:Y4"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="W6:Y6"/>
-    <mergeCell ref="W7:Y7"/>
-    <mergeCell ref="W8:Y8"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="K1:S1"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" copies="0" r:id="rId1"/>

</xml_diff>